<commit_message>
Resolve conflicts: keep local versions
</commit_message>
<xml_diff>
--- a/ServiceNowAutomation/incident.xlsx
+++ b/ServiceNowAutomation/incident.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPI3XY\source\repos\ServiceNowAutomation\ServiceNowAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4D3CD0-B31B-4B8E-9823-C865926EBFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DD6796-2894-4705-86E2-171D5EDCE36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14670" yWindow="4695" windowWidth="21600" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page 1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Number</t>
   </si>
@@ -41,106 +41,10 @@
     <t>Short description</t>
   </si>
   <si>
-    <t>INC2307018</t>
+    <t>INC0100</t>
   </si>
   <si>
-    <t>próbuje zrobić protokół przekazania pojazdu 5793455, otrzymuje komunikat , że taki pojaz nie istnieje i nie mogę wygenerować protokołu</t>
-  </si>
-  <si>
-    <t>INC2318647</t>
-  </si>
-  <si>
-    <t>AM - brak faktur za zamówienia SO. Wygląda na to, że nie ma w systemie faktury z fabryki o numerze 5582898. Prośba o pilne sprawdzenie, bo serwisy nie mogą zamk</t>
-  </si>
-  <si>
-    <t>INC2316792</t>
-  </si>
-  <si>
-    <t>Zmiana kursu bazowego na umowach w Egerii. Zmiana dotyczy umów Leasingu oeracyjnego w EURO, które na dzień 31-12-2025 nie są zakończone.</t>
-  </si>
-  <si>
-    <t>INC2316765</t>
-  </si>
-  <si>
-    <t>Prośba o zmianę adresatów From: DB_SFP SQL Server &lt;sqlserver_db-sfp@scania.pl&gt; 
-obecni:
-sqlserver_db-sfp@scania.pl; Munik Kamil &lt;kamil.munik@scania.com&gt;; Pami</t>
-  </si>
-  <si>
-    <t>INC2316207</t>
-  </si>
-  <si>
-    <t>Brak możliwości przyjęcia zamówienia Nr HU: 2040205584</t>
-  </si>
-  <si>
-    <t>INC2315818</t>
-  </si>
-  <si>
-    <t>Zamówienie o nr. 403879337, a w nim 2 części tj. 2587113, 2643437, w Automaster zamówienie ma status potwierdzone od 05.12.25, pisałem o fakturę do spl. parts i</t>
-  </si>
-  <si>
-    <t>INC2315636</t>
-  </si>
-  <si>
-    <t>Dzień dobry, nie mogę przyjąc na stan paczki nr 2040205611 wg działu części zamiennych FV została wystawina i z ich strony jest wszystko OK, wyszukując część zn</t>
-  </si>
-  <si>
-    <t>INC2315275</t>
-  </si>
-  <si>
-    <t>System BONUS w AM
-Brak mozliwości zgłoszenia do gwarancji sprzedaży autobusów o nr vin 1929806; 1929810; 1929887</t>
-  </si>
-  <si>
-    <t>INC2315182</t>
-  </si>
-  <si>
-    <t>zablokowane konto EGERIA</t>
-  </si>
-  <si>
-    <t>INC2314294</t>
-  </si>
-  <si>
-    <t>Dzień Dobry, zgłaszam problem z RemoveBox. Mechanicy na wyjeździe Assistance mają problem z połączeniem się z nim poprzez tablety, tablet wgl nie widzi sieci wi</t>
-  </si>
-  <si>
-    <t>INC2313593</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Od wczoraj nie można się zalogować do iScala. Przy próbie logowania pojawia się błąd jak w załączniku.
-Żaden plik powiązany z bazą iScala nie działa. Proszę o </t>
-  </si>
-  <si>
-    <t>INC2309978</t>
-  </si>
-  <si>
-    <t>Zbyt wolne działanie komputerów i internetu,  bardzo długo wczytujje aktualizacje  prosze o werywikację .</t>
-  </si>
-  <si>
-    <t>INC2309743</t>
-  </si>
-  <si>
-    <t>Proszę o konfiguracje 2 szt VCI4 o numerze 240267, 240260</t>
-  </si>
-  <si>
-    <t>INC2308990</t>
-  </si>
-  <si>
-    <t>Cześć,
-kolejny raz po otwarciu raportu zamknięte zlecenia nie pojawia się aktualny miesiąc. Raport otwierany jest z BI.
-Często rano odpalają serwisy i nie poj</t>
-  </si>
-  <si>
-    <t>INC2300660</t>
-  </si>
-  <si>
-    <t>Brak możliwości przypisania nowego WCU (S/N: KSA5263015) do nowego serwisu SPL Rokietnica. Do tej pory przypisywałem przez stronę https://sws.scania.com/device,</t>
-  </si>
-  <si>
-    <t>INC2293651</t>
-  </si>
-  <si>
-    <t>cześć, Klient 1118096 poinformował nas o problemie z Ebok. Twierdzi, że ostatnie miesiące faktury ze Scania Polska oraz Scania Finance otrzymywał drogą elektron</t>
+    <t>Brak faktury</t>
   </si>
 </sst>
 </file>
@@ -521,11 +425,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,132 +448,19 @@
     </row>
     <row r="2" spans="1:2" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
+    <row r="3" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:2" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>